<commit_message>
pt_element.erb: Set up basic property-hash processor to output properties in order of hash. Put in some existing tweaks. To do: --Follow property_n[options] hash model for options --Copy in tweaks from element.erb (for *_is_estimated) --Consider allowing to choose more tweaks using options (e.g., putting brackets around not-well-known masses, or not)
</commit_message>
<xml_diff>
--- a/repetitive command builder.xlsx
+++ b/repetitive command builder.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25760" yWindow="660" windowWidth="25440" windowHeight="15240" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="15240" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="pt_element" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>name_origin</t>
   </si>
@@ -86,6 +87,41 @@
   </si>
   <si>
     <t xml:space="preserve">    &lt;span class="pt_"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>atomic_num</t>
+  </si>
+  <si>
+    <t>symbol</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>e_config</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;%= element.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    &lt;div class="pt_"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> %&gt;&lt;/div&gt;
+ </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;% when '</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> %&gt;
+  </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -144,9 +180,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,10 +519,229 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:G20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="3" width="40.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="26">
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1">
+      <c r="A2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="str">
+        <f>CONCATENATE(B$1,$A2,C$1,D$1,$A2,E$1,F$1,$A2,G$1)</f>
+        <v xml:space="preserve"> &lt;% when 'atomic_num %&gt;_x000D_      &lt;div class="pt_"atomic_num"&gt;&lt;%= element.atomic_num %&gt;&lt;/div&gt;_x000D_ </v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="2" customFormat="1">
+      <c r="A3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B20" si="0">CONCATENATE(B$1,$A3,C$1,D$1,$A3,E$1,F$1,$A3,G$1)</f>
+        <v xml:space="preserve"> &lt;% when 'symbol %&gt;_x000D_      &lt;div class="pt_"symbol"&gt;&lt;%= element.symbol %&gt;&lt;/div&gt;_x000D_ </v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="2" customFormat="1">
+      <c r="A4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &lt;% when 'name %&gt;_x000D_      &lt;div class="pt_"name"&gt;&lt;%= element.name %&gt;&lt;/div&gt;_x000D_ </v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &lt;% when 'name_origin %&gt;_x000D_      &lt;div class="pt_"name_origin"&gt;&lt;%= element.name_origin %&gt;&lt;/div&gt;_x000D_ </v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &lt;% when 'group %&gt;_x000D_      &lt;div class="pt_"group"&gt;&lt;%= element.group %&gt;&lt;/div&gt;_x000D_ </v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &lt;% when 'period %&gt;_x000D_      &lt;div class="pt_"period"&gt;&lt;%= element.period %&gt;&lt;/div&gt;_x000D_ </v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &lt;% when 'atomic_weight %&gt;_x000D_      &lt;div class="pt_"atomic_weight"&gt;&lt;%= element.atomic_weight %&gt;&lt;/div&gt;_x000D_ </v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &lt;% when 'atomic_wt_is_mass_number_of_longest_lived_isotope %&gt;_x000D_      &lt;div class="pt_"atomic_wt_is_mass_number_of_longest_lived_isotope"&gt;&lt;%= element.atomic_wt_is_mass_number_of_longest_lived_isotope %&gt;&lt;/div&gt;_x000D_ </v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &lt;% when 'specific_heat_capacity_J_per_gK %&gt;_x000D_      &lt;div class="pt_"specific_heat_capacity_J_per_gK"&gt;&lt;%= element.specific_heat_capacity_J_per_gK %&gt;&lt;/div&gt;_x000D_ </v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &lt;% when 'density_g_per_cm3 %&gt;_x000D_      &lt;div class="pt_"density_g_per_cm3"&gt;&lt;%= element.density_g_per_cm3 %&gt;&lt;/div&gt;_x000D_ </v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &lt;% when 'density_is_estimated %&gt;_x000D_      &lt;div class="pt_"density_is_estimated"&gt;&lt;%= element.density_is_estimated %&gt;&lt;/div&gt;_x000D_ </v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &lt;% when 'melting_point_k %&gt;_x000D_      &lt;div class="pt_"melting_point_k"&gt;&lt;%= element.melting_point_k %&gt;&lt;/div&gt;_x000D_ </v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &lt;% when 'melt_is_estimated %&gt;_x000D_      &lt;div class="pt_"melt_is_estimated"&gt;&lt;%= element.melt_is_estimated %&gt;&lt;/div&gt;_x000D_ </v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &lt;% when 'boiling_point_k %&gt;_x000D_      &lt;div class="pt_"boiling_point_k"&gt;&lt;%= element.boiling_point_k %&gt;&lt;/div&gt;_x000D_ </v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &lt;% when 'boil_is_estimated %&gt;_x000D_      &lt;div class="pt_"boil_is_estimated"&gt;&lt;%= element.boil_is_estimated %&gt;&lt;/div&gt;_x000D_ </v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &lt;% when 'electronegativity %&gt;_x000D_      &lt;div class="pt_"electronegativity"&gt;&lt;%= element.electronegativity %&gt;&lt;/div&gt;_x000D_ </v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &lt;% when 'abundance_mg_per_kg %&gt;_x000D_      &lt;div class="pt_"abundance_mg_per_kg"&gt;&lt;%= element.abundance_mg_per_kg %&gt;&lt;/div&gt;_x000D_ </v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &lt;% when 'abundance_is_upper_limit %&gt;_x000D_      &lt;div class="pt_"abundance_is_upper_limit"&gt;&lt;%= element.abundance_is_upper_limit %&gt;&lt;/div&gt;_x000D_ </v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> &lt;% when 'e_config %&gt;_x000D_      &lt;div class="pt_"e_config"&gt;&lt;%= element.e_config %&gt;&lt;/div&gt;_x000D_ </v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B18"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -656,7 +918,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Repetitive command builder and pt_element.erb: removed capital letters from "specific_heat_capacity_j_per_gk"
</commit_message>
<xml_diff>
--- a/repetitive command builder.xlsx
+++ b/repetitive command builder.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="pt_element" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="original element cell" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>name_origin</t>
   </si>
@@ -107,21 +107,32 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">    &lt;div class="pt_"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> %&gt;&lt;/div&gt;
- </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve"> &lt;% when '</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> %&gt;
+    <t xml:space="preserve">' %&gt;
   </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> %&gt;&lt;/div&gt; </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    &lt;div class='pt_</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>'&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>specific_heat_capacity_j_per_gk</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -180,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -190,6 +201,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -522,7 +534,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -535,22 +547,22 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="26">
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>18</v>
+      <c r="E1" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>25</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1">
@@ -559,7 +571,10 @@
       </c>
       <c r="B2" t="str">
         <f>CONCATENATE(B$1,$A2,C$1,D$1,$A2,E$1,F$1,$A2,G$1)</f>
-        <v xml:space="preserve"> &lt;% when 'atomic_num %&gt;_x000D_      &lt;div class="pt_"atomic_num"&gt;&lt;%= element.atomic_num %&gt;&lt;/div&gt;_x000D_ </v>
+        <v xml:space="preserve"> &lt;% when 'atomic_num' %&gt;_x000D_      &lt;div class='pt_atomic_num'&gt;&lt;%= element.atomic_num %&gt;&lt;/div&gt; </v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="2" customFormat="1">
@@ -568,7 +583,7 @@
       </c>
       <c r="B3" t="str">
         <f t="shared" ref="B3:B20" si="0">CONCATENATE(B$1,$A3,C$1,D$1,$A3,E$1,F$1,$A3,G$1)</f>
-        <v xml:space="preserve"> &lt;% when 'symbol %&gt;_x000D_      &lt;div class="pt_"symbol"&gt;&lt;%= element.symbol %&gt;&lt;/div&gt;_x000D_ </v>
+        <v xml:space="preserve"> &lt;% when 'symbol' %&gt;_x000D_      &lt;div class='pt_symbol'&gt;&lt;%= element.symbol %&gt;&lt;/div&gt; </v>
       </c>
     </row>
     <row r="4" spans="1:7" s="2" customFormat="1">
@@ -577,7 +592,7 @@
       </c>
       <c r="B4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> &lt;% when 'name %&gt;_x000D_      &lt;div class="pt_"name"&gt;&lt;%= element.name %&gt;&lt;/div&gt;_x000D_ </v>
+        <v xml:space="preserve"> &lt;% when 'name' %&gt;_x000D_      &lt;div class='pt_name'&gt;&lt;%= element.name %&gt;&lt;/div&gt; </v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -586,7 +601,7 @@
       </c>
       <c r="B5" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> &lt;% when 'name_origin %&gt;_x000D_      &lt;div class="pt_"name_origin"&gt;&lt;%= element.name_origin %&gt;&lt;/div&gt;_x000D_ </v>
+        <v xml:space="preserve"> &lt;% when 'name_origin' %&gt;_x000D_      &lt;div class='pt_name_origin'&gt;&lt;%= element.name_origin %&gt;&lt;/div&gt; </v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -595,7 +610,7 @@
       </c>
       <c r="B6" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> &lt;% when 'group %&gt;_x000D_      &lt;div class="pt_"group"&gt;&lt;%= element.group %&gt;&lt;/div&gt;_x000D_ </v>
+        <v xml:space="preserve"> &lt;% when 'group' %&gt;_x000D_      &lt;div class='pt_group'&gt;&lt;%= element.group %&gt;&lt;/div&gt; </v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -604,7 +619,7 @@
       </c>
       <c r="B7" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> &lt;% when 'period %&gt;_x000D_      &lt;div class="pt_"period"&gt;&lt;%= element.period %&gt;&lt;/div&gt;_x000D_ </v>
+        <v xml:space="preserve"> &lt;% when 'period' %&gt;_x000D_      &lt;div class='pt_period'&gt;&lt;%= element.period %&gt;&lt;/div&gt; </v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -613,7 +628,7 @@
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> &lt;% when 'atomic_weight %&gt;_x000D_      &lt;div class="pt_"atomic_weight"&gt;&lt;%= element.atomic_weight %&gt;&lt;/div&gt;_x000D_ </v>
+        <v xml:space="preserve"> &lt;% when 'atomic_weight' %&gt;_x000D_      &lt;div class='pt_atomic_weight'&gt;&lt;%= element.atomic_weight %&gt;&lt;/div&gt; </v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -622,16 +637,16 @@
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> &lt;% when 'atomic_wt_is_mass_number_of_longest_lived_isotope %&gt;_x000D_      &lt;div class="pt_"atomic_wt_is_mass_number_of_longest_lived_isotope"&gt;&lt;%= element.atomic_wt_is_mass_number_of_longest_lived_isotope %&gt;&lt;/div&gt;_x000D_ </v>
+        <v xml:space="preserve"> &lt;% when 'atomic_wt_is_mass_number_of_longest_lived_isotope' %&gt;_x000D_      &lt;div class='pt_atomic_wt_is_mass_number_of_longest_lived_isotope'&gt;&lt;%= element.atomic_wt_is_mass_number_of_longest_lived_isotope %&gt;&lt;/div&gt; </v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> &lt;% when 'specific_heat_capacity_J_per_gK %&gt;_x000D_      &lt;div class="pt_"specific_heat_capacity_J_per_gK"&gt;&lt;%= element.specific_heat_capacity_J_per_gK %&gt;&lt;/div&gt;_x000D_ </v>
+        <v xml:space="preserve"> &lt;% when 'specific_heat_capacity_j_per_gk' %&gt;_x000D_      &lt;div class='pt_specific_heat_capacity_j_per_gk'&gt;&lt;%= element.specific_heat_capacity_j_per_gk %&gt;&lt;/div&gt; </v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -640,7 +655,7 @@
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> &lt;% when 'density_g_per_cm3 %&gt;_x000D_      &lt;div class="pt_"density_g_per_cm3"&gt;&lt;%= element.density_g_per_cm3 %&gt;&lt;/div&gt;_x000D_ </v>
+        <v xml:space="preserve"> &lt;% when 'density_g_per_cm3' %&gt;_x000D_      &lt;div class='pt_density_g_per_cm3'&gt;&lt;%= element.density_g_per_cm3 %&gt;&lt;/div&gt; </v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -649,7 +664,7 @@
       </c>
       <c r="B12" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> &lt;% when 'density_is_estimated %&gt;_x000D_      &lt;div class="pt_"density_is_estimated"&gt;&lt;%= element.density_is_estimated %&gt;&lt;/div&gt;_x000D_ </v>
+        <v xml:space="preserve"> &lt;% when 'density_is_estimated' %&gt;_x000D_      &lt;div class='pt_density_is_estimated'&gt;&lt;%= element.density_is_estimated %&gt;&lt;/div&gt; </v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -658,7 +673,7 @@
       </c>
       <c r="B13" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> &lt;% when 'melting_point_k %&gt;_x000D_      &lt;div class="pt_"melting_point_k"&gt;&lt;%= element.melting_point_k %&gt;&lt;/div&gt;_x000D_ </v>
+        <v xml:space="preserve"> &lt;% when 'melting_point_k' %&gt;_x000D_      &lt;div class='pt_melting_point_k'&gt;&lt;%= element.melting_point_k %&gt;&lt;/div&gt; </v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -667,7 +682,7 @@
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> &lt;% when 'melt_is_estimated %&gt;_x000D_      &lt;div class="pt_"melt_is_estimated"&gt;&lt;%= element.melt_is_estimated %&gt;&lt;/div&gt;_x000D_ </v>
+        <v xml:space="preserve"> &lt;% when 'melt_is_estimated' %&gt;_x000D_      &lt;div class='pt_melt_is_estimated'&gt;&lt;%= element.melt_is_estimated %&gt;&lt;/div&gt; </v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -676,7 +691,7 @@
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> &lt;% when 'boiling_point_k %&gt;_x000D_      &lt;div class="pt_"boiling_point_k"&gt;&lt;%= element.boiling_point_k %&gt;&lt;/div&gt;_x000D_ </v>
+        <v xml:space="preserve"> &lt;% when 'boiling_point_k' %&gt;_x000D_      &lt;div class='pt_boiling_point_k'&gt;&lt;%= element.boiling_point_k %&gt;&lt;/div&gt; </v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -685,7 +700,7 @@
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> &lt;% when 'boil_is_estimated %&gt;_x000D_      &lt;div class="pt_"boil_is_estimated"&gt;&lt;%= element.boil_is_estimated %&gt;&lt;/div&gt;_x000D_ </v>
+        <v xml:space="preserve"> &lt;% when 'boil_is_estimated' %&gt;_x000D_      &lt;div class='pt_boil_is_estimated'&gt;&lt;%= element.boil_is_estimated %&gt;&lt;/div&gt; </v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -694,7 +709,7 @@
       </c>
       <c r="B17" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> &lt;% when 'electronegativity %&gt;_x000D_      &lt;div class="pt_"electronegativity"&gt;&lt;%= element.electronegativity %&gt;&lt;/div&gt;_x000D_ </v>
+        <v xml:space="preserve"> &lt;% when 'electronegativity' %&gt;_x000D_      &lt;div class='pt_electronegativity'&gt;&lt;%= element.electronegativity %&gt;&lt;/div&gt; </v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -703,7 +718,7 @@
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> &lt;% when 'abundance_mg_per_kg %&gt;_x000D_      &lt;div class="pt_"abundance_mg_per_kg"&gt;&lt;%= element.abundance_mg_per_kg %&gt;&lt;/div&gt;_x000D_ </v>
+        <v xml:space="preserve"> &lt;% when 'abundance_mg_per_kg' %&gt;_x000D_      &lt;div class='pt_abundance_mg_per_kg'&gt;&lt;%= element.abundance_mg_per_kg %&gt;&lt;/div&gt; </v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -712,7 +727,7 @@
       </c>
       <c r="B19" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> &lt;% when 'abundance_is_upper_limit %&gt;_x000D_      &lt;div class="pt_"abundance_is_upper_limit"&gt;&lt;%= element.abundance_is_upper_limit %&gt;&lt;/div&gt;_x000D_ </v>
+        <v xml:space="preserve"> &lt;% when 'abundance_is_upper_limit' %&gt;_x000D_      &lt;div class='pt_abundance_is_upper_limit'&gt;&lt;%= element.abundance_is_upper_limit %&gt;&lt;/div&gt; </v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -721,7 +736,7 @@
       </c>
       <c r="B20" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> &lt;% when 'e_config %&gt;_x000D_      &lt;div class="pt_"e_config"&gt;&lt;%= element.e_config %&gt;&lt;/div&gt;_x000D_ </v>
+        <v xml:space="preserve"> &lt;% when 'e_config' %&gt;_x000D_      &lt;div class='pt_e_config'&gt;&lt;%= element.e_config %&gt;&lt;/div&gt; </v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added comments to code
</commit_message>
<xml_diff>
--- a/repetitive command builder.xlsx
+++ b/repetitive command builder.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="15240" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25440" windowHeight="15240" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="pt_element" sheetId="2" r:id="rId1"/>
@@ -37,9 +37,6 @@
     <t>atomic_wt_is_mass_number_of_longest_lived_isotope</t>
   </si>
   <si>
-    <t>specific_heat_capacity_J_per_gK</t>
-  </si>
-  <si>
     <t>density_g_per_cm3</t>
   </si>
   <si>
@@ -129,6 +126,10 @@
   </si>
   <si>
     <t>'&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>specific_heat_capacity_j_per_gk</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -533,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -547,39 +548,39 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="26">
       <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1">
       <c r="A2" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" t="str">
         <f>CONCATENATE(B$1,$A2,C$1,D$1,$A2,E$1,F$1,$A2,G$1)</f>
         <v xml:space="preserve"> &lt;% when 'atomic_num' %&gt;_x000D_      &lt;div class='pt_atomic_num'&gt;&lt;%= element.atomic_num %&gt;&lt;/div&gt; </v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="2" customFormat="1">
       <c r="A3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" t="str">
         <f t="shared" ref="B3:B20" si="0">CONCATENATE(B$1,$A3,C$1,D$1,$A3,E$1,F$1,$A3,G$1)</f>
@@ -588,7 +589,7 @@
     </row>
     <row r="4" spans="1:7" s="2" customFormat="1">
       <c r="A4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" si="0"/>
@@ -642,7 +643,7 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
@@ -651,7 +652,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
@@ -660,7 +661,7 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" t="str">
         <f t="shared" si="0"/>
@@ -669,7 +670,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" t="str">
         <f t="shared" si="0"/>
@@ -678,7 +679,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
@@ -687,7 +688,7 @@
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
@@ -696,7 +697,7 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
@@ -705,7 +706,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B17" t="str">
         <f t="shared" si="0"/>
@@ -714,7 +715,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>
@@ -723,7 +724,7 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B19" t="str">
         <f t="shared" si="0"/>
@@ -732,7 +733,7 @@
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" t="str">
         <f t="shared" si="0"/>
@@ -755,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -769,21 +770,21 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="1" customFormat="1">
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -833,16 +834,16 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    &lt;span class="pt_"specific_heat_capacity_J_per_gK"&gt;specific_heat_capacity_J_per_gK: &lt;%= element.specific_heat_capacity_J_per_gK %&gt;&lt;/span&gt;&lt;br&gt;</v>
+        <v xml:space="preserve">    &lt;span class="pt_"specific_heat_capacity_j_per_gk"&gt;specific_heat_capacity_j_per_gk: &lt;%= element.specific_heat_capacity_j_per_gk %&gt;&lt;/span&gt;&lt;br&gt;</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="0"/>
@@ -851,7 +852,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="0"/>
@@ -860,7 +861,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="0"/>
@@ -869,7 +870,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" t="str">
         <f t="shared" si="0"/>
@@ -878,7 +879,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" t="str">
         <f t="shared" si="0"/>
@@ -887,7 +888,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="0"/>
@@ -896,7 +897,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="0"/>
@@ -905,7 +906,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="0"/>
@@ -914,7 +915,7 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" t="str">
         <f t="shared" si="0"/>
@@ -923,7 +924,7 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="0"/>

</xml_diff>